<commit_message>
Adicionando a implementação da API no backlog do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Backlog Nunca É So Café.xlsx
+++ b/Documentação/Backlog Nunca É So Café.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagne\OneDrive\Documentos\Projetos\Repósitórios GitHub\Pessoal\Nunca_E_So_Cafe\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F578D3FE-D638-49A3-8CDF-BCFCA2764E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D745E3A6-BD32-434C-A339-B415FD5D0C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66147315-2B54-425F-938E-0D50812079F7}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>Requisito</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Apresentação do projeto para equipe sócio emocional e equipe técnica</t>
+  </si>
+  <si>
+    <t>Implementação da API</t>
+  </si>
+  <si>
+    <t>Implementação da API disponibilizada para funcionamento do site</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,7 +310,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,9 +328,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45221.61838900463" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{F2D3C033-5BC4-40F8-8DF4-4314C3FF7789}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45221.882263310188" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{F2D3C033-5BC4-40F8-8DF4-4314C3FF7789}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I17" sheet="Backlog"/>
+    <worksheetSource ref="A1:I18" sheet="Backlog"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Área" numFmtId="0">
@@ -376,8 +381,8 @@
     </cacheField>
     <cacheField name="Sprint" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1" count="2">
+        <n v="1"/>
         <m/>
-        <n v="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -411,7 +416,7 @@
     <s v="Funcional"/>
     <s v="Importante"/>
     <n v="2"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -422,7 +427,7 @@
     <s v="Funcional"/>
     <s v="Importante"/>
     <n v="2"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
@@ -433,7 +438,7 @@
     <s v="Funcional"/>
     <s v="Essencial"/>
     <n v="2"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -444,7 +449,7 @@
     <s v="Funcional"/>
     <s v="Desejável"/>
     <n v="3"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -455,7 +460,7 @@
     <s v="Não Funcional"/>
     <s v="Importante"/>
     <n v="2"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -466,7 +471,7 @@
     <s v="Não Funcional"/>
     <s v="Importante"/>
     <n v="3"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
@@ -477,7 +482,7 @@
     <s v="Funcional"/>
     <s v="Essencial"/>
     <n v="2"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
@@ -488,7 +493,7 @@
     <s v="Funcional"/>
     <s v="Essencial"/>
     <n v="2"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -499,7 +504,7 @@
     <s v="Não Funcional"/>
     <s v="Essencial"/>
     <n v="2"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -510,7 +515,7 @@
     <m/>
     <s v="Essencial"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -521,7 +526,7 @@
     <m/>
     <s v="Essencial"/>
     <n v="1"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -532,7 +537,7 @@
     <m/>
     <s v="Desejável"/>
     <n v="3"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -543,7 +548,7 @@
     <m/>
     <s v="Essencial"/>
     <n v="1"/>
-    <x v="1"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -565,13 +570,13 @@
     <m/>
     <s v="Essencial"/>
     <n v="3"/>
-    <x v="0"/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CA5A4CD-0049-4CF7-BE5C-D5166CAA1C7E}" name="Tabela dinâmica2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CA5A4CD-0049-4CF7-BE5C-D5166CAA1C7E}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -612,8 +617,8 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="3">
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1003,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0864F8-286A-4F77-A735-687153E69A69}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,29 +1327,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" s="3">
-        <v>5</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G12" t="s">
         <v>38</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1352,16 +1356,16 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="3">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" t="s">
@@ -1370,29 +1374,32 @@
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="3">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,74 +1407,98 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E15" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F16" s="3"/>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E18" s="3">
         <v>13</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>38</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>3</v>
       </c>
     </row>
@@ -1480,7 +1511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A2327F-FA36-477F-B924-C7B3897C7B56}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1524,11 +1557,10 @@
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="C5">
         <v>13</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5">
         <v>13</v>
       </c>
     </row>
@@ -1536,11 +1568,10 @@
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9">
+      <c r="D6">
         <v>5</v>
       </c>
     </row>
@@ -1548,11 +1579,10 @@
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7">
         <v>8</v>
       </c>
     </row>
@@ -1560,11 +1590,10 @@
       <c r="A8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8">
         <v>5</v>
       </c>
     </row>
@@ -1572,11 +1601,10 @@
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9">
+      <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9">
         <v>5</v>
       </c>
     </row>
@@ -1584,11 +1612,10 @@
       <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9">
+      <c r="C10">
         <v>21</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10">
         <v>21</v>
       </c>
     </row>
@@ -1596,11 +1623,10 @@
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9">
+      <c r="C11">
         <v>21</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11">
         <v>21</v>
       </c>
     </row>
@@ -1608,11 +1634,10 @@
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9">
+      <c r="D12">
         <v>8</v>
       </c>
     </row>
@@ -1620,11 +1645,10 @@
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9">
+      <c r="B13">
         <v>13</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13">
         <v>13</v>
       </c>
     </row>
@@ -1632,11 +1656,10 @@
       <c r="A14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>8</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9">
+      <c r="D14">
         <v>8</v>
       </c>
     </row>
@@ -1644,11 +1667,10 @@
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9">
+      <c r="C15">
         <v>8</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15">
         <v>8</v>
       </c>
     </row>
@@ -1656,11 +1678,10 @@
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9">
+      <c r="C16">
         <v>13</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16">
         <v>13</v>
       </c>
     </row>
@@ -1668,11 +1689,10 @@
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>13</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>13</v>
       </c>
     </row>
@@ -1680,11 +1700,10 @@
       <c r="A18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9">
+      <c r="D18">
         <v>8</v>
       </c>
     </row>
@@ -1692,11 +1711,10 @@
       <c r="A19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9">
+      <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19">
         <v>5</v>
       </c>
     </row>
@@ -1704,11 +1722,10 @@
       <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9">
+      <c r="C20">
         <v>5</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>5</v>
       </c>
     </row>
@@ -1716,13 +1733,13 @@
       <c r="A21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="9">
-        <v>29</v>
-      </c>
-      <c r="C21" s="9">
-        <v>130</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="B21">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <v>112</v>
+      </c>
+      <c r="D21">
         <v>159</v>
       </c>
     </row>
@@ -1736,7 +1753,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:K16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1771,7 @@
       </c>
       <c r="B1" s="2">
         <f>SUM(Backlog!E:E)</f>
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>6</v>
@@ -1784,11 +1801,11 @@
       </c>
       <c r="E2">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="F2" s="2">
         <f>B1-E2</f>
-        <v>127.2</v>
+        <v>137.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1797,18 +1814,18 @@
       </c>
       <c r="B3">
         <f>B1/B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="F3" s="2">
         <f>F2-E3</f>
-        <v>95.4</v>
+        <v>103.19999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1817,11 +1834,11 @@
       </c>
       <c r="E4">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F6" si="0">F3-E4</f>
-        <v>63.600000000000009</v>
+        <v>68.799999999999983</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,11 +1847,11 @@
       </c>
       <c r="E5">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>31.800000000000008</v>
+        <v>34.399999999999984</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1843,7 +1860,7 @@
       </c>
       <c r="E6">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>31.8</v>
+        <v>34.4</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Adicionando tela Inicial, Atualização Backlog
</commit_message>
<xml_diff>
--- a/Documentação/Backlog Nunca É So Café.xlsx
+++ b/Documentação/Backlog Nunca É So Café.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagne\OneDrive\Documentos\Projetos\Repósitórios GitHub\Pessoal\Nunca_E_So_Cafe\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D745E3A6-BD32-434C-A339-B415FD5D0C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95473862-6E79-453C-8A15-B79BCC89FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66147315-2B54-425F-938E-0D50812079F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{66147315-2B54-425F-938E-0D50812079F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabela Dinamica" sheetId="4" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="5" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Tabelas para calculo" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t>Requisito</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Pagina de Usuário</t>
   </si>
   <si>
-    <t>Pagina com nome do usuário, processo preferido, local para seleção de interesses</t>
-  </si>
-  <si>
     <t>Banco de dados</t>
   </si>
   <si>
@@ -181,12 +178,6 @@
     <t>Validação de senha e email</t>
   </si>
   <si>
-    <t>Validação processo</t>
-  </si>
-  <si>
-    <t>Validação do processo escolido no cadastro entre os apresentados no site</t>
-  </si>
-  <si>
     <t>Tamnho do projeto</t>
   </si>
   <si>
@@ -205,9 +196,6 @@
     <t>Faltam</t>
   </si>
   <si>
-    <t>(Tudo)</t>
-  </si>
-  <si>
     <t>Rótulos de Linha</t>
   </si>
   <si>
@@ -245,6 +233,27 @@
   </si>
   <si>
     <t>Implementação da API disponibilizada para funcionamento do site</t>
+  </si>
+  <si>
+    <t>Pagina Receitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversas receitas que utilizam café como ingrediente </t>
+  </si>
+  <si>
+    <t>Pagina com nome do usuário, local para contato, fontes e caminhos para pesquisas ligadas ao interesse do usuario</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos</t>
+  </si>
+  <si>
+    <t>Planilha contendo os ricos do projeto e estratégias para contornalos.</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,37 +338,34 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45221.882263310188" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{F2D3C033-5BC4-40F8-8DF4-4314C3FF7789}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45230.064569560185" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="18" xr:uid="{9475D277-7F79-4C2D-8B4A-C754BD42ED04}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I18" sheet="Backlog"/>
+    <worksheetSource ref="A1:I19" sheet="Backlog"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Área" numFmtId="0">
-      <sharedItems count="4">
-        <s v="Site"/>
-        <s v="Site "/>
-        <s v="Projeto"/>
-        <s v="Projeto "/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Requisito" numFmtId="0">
-      <sharedItems count="16">
+      <sharedItems count="18">
+        <s v="Backlog do projeto"/>
+        <s v="Documentação do projeto"/>
+        <s v="Diagrama de negócio"/>
+        <s v="Trello"/>
+        <s v="Apresentação"/>
+        <s v="Criação do logo"/>
+        <s v="Planilha de Riscos"/>
         <s v="Pagina Inicial"/>
         <s v="Pagina História"/>
         <s v="Pagina Processos"/>
         <s v="Tela de login"/>
         <s v="Recuperação de senha"/>
         <s v="Validação de senha e email"/>
-        <s v="Validação processo"/>
+        <s v="Banco de dados"/>
+        <s v="Implementação da API"/>
+        <s v="Pagina Receitas"/>
         <s v="Tela de cadastro"/>
         <s v="Pagina de Usuário"/>
-        <s v="Banco de dados"/>
-        <s v="Backlog do projeto"/>
-        <s v="Documentação do projeto"/>
-        <s v="Diagrama de negócio"/>
-        <s v="Trello"/>
-        <s v="Criação do logo"/>
-        <s v="Apresentação"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Partes" numFmtId="0">
@@ -374,15 +381,22 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Classificação" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="3">
+        <s v="Essencial"/>
+        <s v="Desejável"/>
+        <s v="Importante"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Prioridade" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
     </cacheField>
     <cacheField name="Sprint" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1" count="2">
-        <n v="1"/>
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="5">
+        <s v="Sprint 1"/>
         <m/>
+        <s v="Sprint 2"/>
+        <n v="1" u="1"/>
+        <n v="2" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -395,217 +409,233 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="18">
   <r>
+    <s v="Projeto"/>
     <x v="0"/>
+    <s v="Tarefas, descrição, tamanho do requisito, classificação, prioridade e Sprint"/>
+    <s v="P"/>
+    <n v="5"/>
+    <m/>
     <x v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Projeto"/>
+    <x v="1"/>
+    <s v="Contexto, objetivo, justificativa, escopo,  requisitos, macro cronograma, premissas, restrições, riscos e partes interessadas"/>
+    <s v="GG"/>
+    <n v="21"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Projeto"/>
+    <x v="2"/>
+    <s v="Diagrama explicando o funcionamento do negócio"/>
+    <s v="P"/>
+    <n v="5"/>
+    <m/>
+    <x v="1"/>
+    <n v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Projeto"/>
+    <x v="3"/>
+    <s v="Backlog na ferramenta, organização de datas, acompanhamento do projeto"/>
+    <s v="M"/>
+    <n v="8"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Projeto"/>
+    <x v="4"/>
+    <s v="Apresentação do projeto para equipe sócio emocional e equipe técnica"/>
+    <s v="G"/>
+    <n v="13"/>
+    <m/>
+    <x v="0"/>
+    <n v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Projeto "/>
+    <x v="5"/>
+    <s v="Criação do logo do site"/>
+    <s v="P"/>
+    <n v="5"/>
+    <m/>
+    <x v="2"/>
+    <n v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Projeto "/>
+    <x v="6"/>
+    <s v="Planilha contendo os ricos do projeto e estratégias para contornalos."/>
+    <s v="M"/>
+    <n v="8"/>
+    <m/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Site"/>
+    <x v="7"/>
     <s v="O que é café, vantagens e desvantagens, resumo do projeto"/>
     <s v="G"/>
     <n v="13"/>
     <s v="Funcional"/>
-    <s v="Essencial"/>
+    <x v="0"/>
     <n v="1"/>
-    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="1"/>
+    <s v="Site"/>
+    <x v="8"/>
     <s v="Resumo da história do café"/>
     <s v="M"/>
     <n v="8"/>
     <s v="Funcional"/>
-    <s v="Importante"/>
+    <x v="2"/>
     <n v="2"/>
     <x v="0"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="2"/>
+    <s v="Site"/>
+    <x v="9"/>
     <s v="Resumo dos diversos processos de produção de café"/>
     <s v="M"/>
     <n v="8"/>
     <s v="Funcional"/>
-    <s v="Importante"/>
+    <x v="2"/>
     <n v="2"/>
     <x v="0"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="3"/>
+    <s v="Site"/>
+    <x v="10"/>
     <s v="Pop-Up com Área de login e senha, botão para entrar e link par cadastro "/>
     <s v="G"/>
     <n v="13"/>
     <s v="Funcional"/>
-    <s v="Essencial"/>
+    <x v="0"/>
+    <n v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Site"/>
+    <x v="11"/>
+    <s v="Link para recuperação de senha"/>
+    <s v="M"/>
+    <n v="8"/>
+    <s v="Funcional"/>
+    <x v="1"/>
+    <n v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Site"/>
+    <x v="12"/>
+    <s v="Validação da criação de senha e do email de acordo com as regras estabelecidas"/>
+    <s v="P"/>
+    <n v="5"/>
+    <s v="Não Funcional"/>
+    <x v="2"/>
+    <n v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Site"/>
+    <x v="13"/>
+    <s v="Modelagem lógica, script de criação das tabelas, inserção e seleção de dados"/>
+    <s v="M"/>
+    <n v="8"/>
+    <s v="Não Funcional"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="1"/>
   </r>
   <r>
+    <s v="Site"/>
+    <x v="14"/>
+    <s v="Implementação da API disponibilizada para funcionamento do site"/>
+    <s v="G"/>
+    <n v="13"/>
+    <s v="Não Funcional"/>
     <x v="0"/>
-    <x v="4"/>
-    <s v="Link para recuperação de senha"/>
-    <s v="M"/>
-    <n v="8"/>
-    <s v="Funcional"/>
-    <s v="Desejável"/>
     <n v="3"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="5"/>
-    <s v="Validação da criação de senha e do email de acordo com as regras estabelecidas"/>
-    <s v="p"/>
-    <n v="5"/>
-    <s v="Não Funcional"/>
-    <s v="Importante"/>
-    <n v="2"/>
+    <s v="Site"/>
+    <x v="15"/>
+    <s v="Diversas receitas que utilizam café como ingrediente "/>
+    <s v="M"/>
+    <n v="8"/>
+    <s v="Funcional"/>
     <x v="1"/>
+    <n v="3"/>
+    <x v="2"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="6"/>
-    <s v="Validação do processo escolido no cadastro entre os apresentados no site"/>
-    <s v="p"/>
-    <n v="5"/>
-    <s v="Não Funcional"/>
-    <s v="Importante"/>
-    <n v="3"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="7"/>
+    <s v="Site "/>
+    <x v="16"/>
     <s v="Área para email, nome, sobrenome, CEP,numero do logradouro, complemento, processo de café preferido, senha e confirmação de senha"/>
     <s v="G"/>
     <n v="13"/>
     <s v="Funcional"/>
-    <s v="Essencial"/>
+    <x v="0"/>
     <n v="2"/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="8"/>
-    <s v="Pagina com nome do usuário, processo preferido, local para seleção de interesses"/>
+    <s v="Site "/>
+    <x v="17"/>
+    <s v="Pagina com nome do usuário, local para contato, fontes e caminhos para pesquisas ligadas ao interesse do usuario"/>
     <s v="GG"/>
     <n v="21"/>
     <s v="Funcional"/>
-    <s v="Essencial"/>
+    <x v="0"/>
     <n v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="9"/>
-    <s v="Modelagem lógica, script de criação das tabelas, inserção e seleção de dados"/>
-    <s v="M"/>
-    <n v="8"/>
-    <s v="Não Funcional"/>
-    <s v="Essencial"/>
-    <n v="2"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="10"/>
-    <s v="Tarefas, descrição, tamanho do requisito, classificação, prioridade e Sprint"/>
-    <s v="p"/>
-    <n v="5"/>
-    <m/>
-    <s v="Essencial"/>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="11"/>
-    <s v="Contexto, objetivo, justificativa, escopo,  requisitos, macro cronograma, premissas, restrições, riscos e partes interessadas"/>
-    <s v="GG"/>
-    <n v="21"/>
-    <m/>
-    <s v="Essencial"/>
-    <n v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="12"/>
-    <s v="Diagrama explicando o funcionamento do negócio"/>
-    <s v="p"/>
-    <n v="5"/>
-    <m/>
-    <s v="Desejável"/>
-    <n v="3"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="13"/>
-    <s v="Backlog na ferramenta, organização de datas, acompanhamento do projeto"/>
-    <s v="M"/>
-    <n v="8"/>
-    <m/>
-    <s v="Essencial"/>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="14"/>
-    <s v="Criação do logo do site"/>
-    <s v="p"/>
-    <n v="5"/>
-    <m/>
-    <s v="Importante"/>
-    <n v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="15"/>
-    <s v="Apresentação do projeto para equipe sócio emocional e equipe técnica"/>
-    <s v="G"/>
-    <n v="13"/>
-    <m/>
-    <s v="Essencial"/>
-    <n v="3"/>
     <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CA5A4CD-0049-4CF7-BE5C-D5166CAA1C7E}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EF14FE4-3550-4E69-AE4C-C03FB3612E63}" name="Tabela dinâmica1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:E23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="3"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="19">
+        <item x="4"/>
         <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="17">
-        <item x="15"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="3"/>
         <item x="13"/>
         <item x="5"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="15"/>
         <item x="6"/>
+        <item x="11"/>
+        <item x="16"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -613,12 +643,22 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="1" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="3">
+      <items count="6">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -626,7 +666,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
@@ -675,6 +715,12 @@
     <i>
       <x v="15"/>
     </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -682,20 +728,20 @@
   <colFields count="1">
     <field x="8"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
-      <x/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
-  <pageFields count="1">
-    <pageField fld="0" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Fibonnaci" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
@@ -1007,11 +1053,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B4FCC4-6205-4A3C-845C-54647A2D5C74}">
+  <dimension ref="A3:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="9">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="9">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="9">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9">
+        <v>21</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
+        <v>8</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9">
+        <v>8</v>
+      </c>
+      <c r="E16" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="9">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="9">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
+        <v>13</v>
+      </c>
+      <c r="E20" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9">
+        <v>8</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="9">
+        <v>97</v>
+      </c>
+      <c r="C23" s="9">
+        <v>34</v>
+      </c>
+      <c r="D23" s="9">
+        <v>52</v>
+      </c>
+      <c r="E23" s="9">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0864F8-286A-4F77-A735-687153E69A69}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,10 +1387,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
@@ -1058,138 +1401,124 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="3">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" t="s">
         <v>39</v>
       </c>
       <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="3">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1197,106 +1526,109 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3">
         <v>5</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
       <c r="H8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>38</v>
       </c>
       <c r="H10">
         <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1304,25 +1636,28 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3">
         <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>38</v>
       </c>
       <c r="H11">
         <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1330,420 +1665,225 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3">
         <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
       <c r="H12">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="3">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3"/>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3">
-        <v>21</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" t="s">
         <v>38</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" s="3">
-        <v>5</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E16" s="3">
-        <v>8</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" s="3">
-        <v>5</v>
       </c>
       <c r="G17" t="s">
         <v>39</v>
       </c>
       <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3">
         <v>13</v>
       </c>
+      <c r="F18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="3">
+        <v>21</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A2327F-FA36-477F-B924-C7B3897C7B56}">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>21</v>
-      </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>13</v>
-      </c>
-      <c r="D16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21">
-        <v>47</v>
-      </c>
-      <c r="C21">
-        <v>112</v>
-      </c>
-      <c r="D21">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I19">
+    <sortCondition ref="A13:A19"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1753,7 +1893,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,31 +1907,31 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2">
         <f>SUM(Backlog!E:E)</f>
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1801,31 +1941,31 @@
       </c>
       <c r="E2">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="F2" s="2">
         <f>B1-E2</f>
-        <v>137.6</v>
+        <v>146.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <f>B1/B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="F3" s="2">
         <f>F2-E3</f>
-        <v>103.19999999999999</v>
+        <v>109.80000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1834,11 +1974,11 @@
       </c>
       <c r="E4">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F6" si="0">F3-E4</f>
-        <v>68.799999999999983</v>
+        <v>73.200000000000017</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1847,11 +1987,11 @@
       </c>
       <c r="E5">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>34.399999999999984</v>
+        <v>36.600000000000016</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1860,7 +2000,7 @@
       </c>
       <c r="E6">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>34.4</v>
+        <v>36.6</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
@@ -2024,20 +2164,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2059,14 +2199,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B25C3F-8B7C-4CC2-B5FC-BF1C69CB6358}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6CAA2B-D6B3-4BC2-AE0B-FFB3EDAE6792}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2080,4 +2212,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B25C3F-8B7C-4CC2-B5FC-BF1C69CB6358}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adicionando html e css tela de login
</commit_message>
<xml_diff>
--- a/Documentação/Backlog Nunca É So Café.xlsx
+++ b/Documentação/Backlog Nunca É So Café.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagne\OneDrive\Documentos\Projetos\Repósitórios GitHub\Pessoal\Nunca_E_So_Cafe\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95473862-6E79-453C-8A15-B79BCC89FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5573CEC4-3B3A-43C0-B686-2A109C71425F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{66147315-2B54-425F-938E-0D50812079F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{66147315-2B54-425F-938E-0D50812079F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="5" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="1" r:id="rId2"/>
-    <sheet name="Tabelas para calculo" sheetId="2" r:id="rId3"/>
+    <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Documentação" sheetId="6" r:id="rId2"/>
+    <sheet name="Tabela dinamica" sheetId="5" r:id="rId3"/>
+    <sheet name="Tabelas para calculo" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="75">
   <si>
     <t>Requisito</t>
   </si>
@@ -254,13 +255,25 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Backlog do Projeto</t>
+  </si>
+  <si>
+    <t>Site e sistema</t>
+  </si>
+  <si>
+    <t>Cadastro de Dissciplinas</t>
+  </si>
+  <si>
+    <t>Cadastro colentando dados das diversar áreas do conhecimento com dificuldades e interesses do usuário.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +281,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +309,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -301,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,7 +352,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,7 +391,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="vagne" refreshedDate="45230.064569560185" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="18" xr:uid="{9475D277-7F79-4C2D-8B4A-C754BD42ED04}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I19" sheet="Backlog"/>
+    <worksheetSource ref="A1:I20" sheet="Backlog"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Área" numFmtId="0">
@@ -612,7 +663,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EF14FE4-3550-4E69-AE4C-C03FB3612E63}" name="Tabela dinâmica1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EF14FE4-3550-4E69-AE4C-C03FB3612E63}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1053,308 +1104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B4FCC4-6205-4A3C-845C-54647A2D5C74}">
-  <dimension ref="A3:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0864F8-286A-4F77-A735-687153E69A69}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="9">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="9">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
-        <v>5</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="9">
-        <v>21</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="9">
-        <v>13</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="9">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9">
-        <v>8</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9">
-        <v>13</v>
-      </c>
-      <c r="E14" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9">
-        <v>8</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9">
-        <v>8</v>
-      </c>
-      <c r="E16" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="9">
-        <v>8</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="9">
-        <v>8</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9">
-        <v>13</v>
-      </c>
-      <c r="E19" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9">
-        <v>13</v>
-      </c>
-      <c r="E20" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9">
-        <v>8</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9">
-        <v>5</v>
-      </c>
-      <c r="E22" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="9">
-        <v>97</v>
-      </c>
-      <c r="C23" s="9">
-        <v>34</v>
-      </c>
-      <c r="D23" s="9">
-        <v>52</v>
-      </c>
-      <c r="E23" s="9">
-        <v>183</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0864F8-286A-4F77-A735-687153E69A69}">
-  <dimension ref="A1:I19"/>
-  <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1566,7 @@
       <c r="E17" s="3">
         <v>8</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G17" t="s">
@@ -1827,31 +1581,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E18" s="3">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H18">
         <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1859,16 +1610,16 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>35</v>
@@ -1879,16 +1630,847 @@
       <c r="H19">
         <v>2</v>
       </c>
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="3">
+        <v>21</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I19">
-    <sortCondition ref="A13:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I20">
+    <sortCondition ref="A13:A20"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93E01FE-78BC-4176-B22A-A9BA0401778A}">
+  <dimension ref="A1:V29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="13"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R17" s="1"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="16"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="R19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R26" s="1"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R27" s="1"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R28" s="1"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R29" s="1"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P12:V29">
+    <sortCondition descending="1" ref="P17:P29"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A18:E18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B4FCC4-6205-4A3C-845C-54647A2D5C74}">
+  <dimension ref="A3:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23">
+        <v>97</v>
+      </c>
+      <c r="C23">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>52</v>
+      </c>
+      <c r="E23">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A7158F-9192-4DE0-A159-9689B51E7B7D}">
   <dimension ref="A1:H25"/>
   <sheetViews>
@@ -1911,7 +2493,7 @@
       </c>
       <c r="B1" s="2">
         <f>SUM(Backlog!E:E)</f>
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>6</v>
@@ -1941,11 +2523,11 @@
       </c>
       <c r="E2">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F2" s="2">
         <f>B1-E2</f>
-        <v>146.4</v>
+        <v>163.19999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1954,18 +2536,18 @@
       </c>
       <c r="B3">
         <f>B1/B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F3" s="2">
         <f>F2-E3</f>
-        <v>109.80000000000001</v>
+        <v>122.39999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1974,11 +2556,11 @@
       </c>
       <c r="E4">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F6" si="0">F3-E4</f>
-        <v>73.200000000000017</v>
+        <v>81.599999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1987,11 +2569,11 @@
       </c>
       <c r="E5">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>36.600000000000016</v>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2000,7 +2582,7 @@
       </c>
       <c r="E6">
         <f>'Tabelas para calculo'!B1/'Tabelas para calculo'!B2</f>
-        <v>36.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
@@ -2164,20 +2746,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2199,6 +2781,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B25C3F-8B7C-4CC2-B5FC-BF1C69CB6358}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D6CAA2B-D6B3-4BC2-AE0B-FFB3EDAE6792}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2212,12 +2802,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B25C3F-8B7C-4CC2-B5FC-BF1C69CB6358}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>